<commit_message>
Add old format massBay concatenation files and code
</commit_message>
<xml_diff>
--- a/data/SeaGrant-TA_DIC-MassBayData/ToRies_Labprocessed2019_sharedSeaGlass.xlsx
+++ b/data/SeaGrant-TA_DIC-MassBayData/ToRies_Labprocessed2019_sharedSeaGlass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/becklabash/Desktop/Sea Grant/data/SeaGrant-TA_DIC-MassBayData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/becklabash/Desktop/SeaGrant/data/SeaGrant-TA_DIC-MassBayData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54884698-3067-C14D-9C90-EB9050029ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFAD6E9-F6E5-C349-B30F-EE77E015E94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="12340" windowWidth="33600" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2120" windowWidth="33600" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="4120" yWindow="3040" windowWidth="10000" windowHeight="8140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
@@ -1736,7 +1736,7 @@
   <dimension ref="A1:AL110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <pane xSplit="4" ySplit="1" topLeftCell="AW2" activePane="bottomRight" state="frozen"/>

</xml_diff>